<commit_message>
storage model infeasible but with an existing solution: issue to be identified
</commit_message>
<xml_diff>
--- a/default/4_sut_multi_year_hourly/concept.xlsx
+++ b/default/4_sut_multi_year_hourly/concept.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\4_sut_multi_year_hourly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA12BCE8-E3B2-424E-B300-1B19028F9842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B92993-10F7-40CC-9D04-38AD45EAB8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
   </bookViews>
   <sheets>
     <sheet name="hours" sheetId="6" r:id="rId1"/>
+    <sheet name="storage" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">hours!$H$38:$I$40,hours!$H$42:$I$44,hours!$L$38:$M$40,hours!$L$42:$M$44,hours!$L$47:$N$48,hours!$H$47:$J$48,hours!$L$73:$N$74</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">storage!$H$34:$I$38,storage!$K$34:$M$38</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">hours!$AM$9:$AN$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">storage!$Z$8:$AD$8</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">storage!$O$34:$O$38</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">hours!$N$47:$N$48</definedName>
     <definedName name="solver_lhs12" localSheetId="0" hidden="1">hours!$L$38:$M$40</definedName>
     <definedName name="solver_lhs13" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
@@ -36,19 +48,33 @@
     <definedName name="solver_lhs17" localSheetId="0" hidden="1">hours!$L$38:$M$40</definedName>
     <definedName name="solver_lhs18" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">hours!$AM$14:$AN$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">storage!$Z$10:$AD$11</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">hours!$AP$9:$AR$9</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">storage!$K$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">hours!$AT$9:$AV$9</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">storage!$K$34:$L$38</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">hours!$AP$14:$AR$15</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">hours!$AT$14:$AV$15</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">storage!$H$34:$I$38</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">hours!$AX$9:$AY$9</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">storage!$O$29</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">hours!$AX$14:$AY$15</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">hours!$L$38:$M$40</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">14</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">10</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">hours!$Q$17</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">storage!$O$13</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">3</definedName>
@@ -58,15 +84,25 @@
     <definedName name="solver_rel17" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel18" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">hours!$L$55:$M$57</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">storage!$M$31</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">hours!$N$58:$N$59</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">hours!$L$62:$M$64</definedName>
     <definedName name="solver_rhs13" localSheetId="0" hidden="1">hours!$L$66:$M$68</definedName>
@@ -76,20 +112,35 @@
     <definedName name="solver_rhs17" localSheetId="0" hidden="1">hours!$L$62:$M$64</definedName>
     <definedName name="solver_rhs18" localSheetId="0" hidden="1">hours!$L$66:$M$68</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">storage!$K$48:$L$52</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">storage!$K$41:$L$45</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">storage!$M$30</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">storage!$M$45</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">storage!$O$26</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">hours!$L$51:$M$53</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">storage!$O$27</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -112,7 +163,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -134,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="101">
   <si>
     <t>flows</t>
   </si>
@@ -350,18 +401,106 @@
   </si>
   <si>
     <t>Q_agg_h - Y_h'-u_h*X_h' - u_y*X_y'*dp.t_y'/n_periods = 0</t>
+  </si>
+  <si>
+    <t>State of charge</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>Thh</t>
+  </si>
+  <si>
+    <t>EE by Coal</t>
+  </si>
+  <si>
+    <t>EE by PV</t>
+  </si>
+  <si>
+    <t>h.4</t>
+  </si>
+  <si>
+    <t>h.5</t>
+  </si>
+  <si>
+    <t>LF max</t>
+  </si>
+  <si>
+    <t>LF min</t>
+  </si>
+  <si>
+    <t>soc min</t>
+  </si>
+  <si>
+    <t>soc max</t>
+  </si>
+  <si>
+    <t>soc start</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>X max</t>
+  </si>
+  <si>
+    <t>C_start</t>
+  </si>
+  <si>
+    <t>X min</t>
+  </si>
+  <si>
+    <t>Q_agg</t>
+  </si>
+  <si>
+    <t>U=u*X_h'</t>
+  </si>
+  <si>
+    <t>Y_h</t>
+  </si>
+  <si>
+    <t>Qagg-U-Y_h==0</t>
+  </si>
+  <si>
+    <t>X'-d*Q_h' == 0</t>
+  </si>
+  <si>
+    <t>soc end</t>
+  </si>
+  <si>
+    <t>SOC start</t>
+  </si>
+  <si>
+    <t>SOC end</t>
+  </si>
+  <si>
+    <t>SOC max</t>
+  </si>
+  <si>
+    <t>SOC min</t>
+  </si>
+  <si>
+    <t>c/d max rate</t>
+  </si>
+  <si>
+    <t>c/d absolute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +527,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -569,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -586,7 +731,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -597,14 +742,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,11 +1044,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6AD6BB-FBFC-41C7-8351-5C5E95720645}">
   <dimension ref="A1:AZ92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="Z7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,15 +1681,8 @@
       <c r="AN16" s="8">
         <v>0</v>
       </c>
-      <c r="AP16" s="29"/>
-      <c r="AQ16" s="29"/>
-      <c r="AR16" s="29"/>
-      <c r="AS16" s="29"/>
-      <c r="AT16" s="29"/>
-      <c r="AU16" s="29"/>
-      <c r="AV16" s="29"/>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>47</v>
       </c>
@@ -1560,7 +1710,7 @@
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>48</v>
       </c>
@@ -1584,7 +1734,7 @@
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -1601,7 +1751,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -1612,7 +1762,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -1626,7 +1776,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1634,26 +1784,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="N24" s="1">
         <v>1</v>
       </c>
-      <c r="AW24" s="25"/>
-      <c r="AX24" s="25"/>
-      <c r="AY24" s="25"/>
-      <c r="AZ24" s="25"/>
-    </row>
-    <row r="25" spans="1:52" s="25" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N25"/>
-      <c r="AW25"/>
-      <c r="AX25"/>
-      <c r="AY25"/>
-      <c r="AZ25"/>
-    </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:27" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>30</v>
       </c>
@@ -1670,7 +1810,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>31</v>
       </c>
@@ -1681,7 +1821,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -1695,7 +1835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1703,7 +1843,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1711,7 +1851,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N31" s="11" t="s">
         <v>66</v>
       </c>
@@ -1719,14 +1859,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="F32" t="s">
         <v>33</v>
       </c>
-      <c r="N32" s="32">
+      <c r="N32" s="30">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
@@ -1738,7 +1878,7 @@
       <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="N33" s="32">
+      <c r="N33" s="30">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
@@ -1750,7 +1890,7 @@
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="32">
+      <c r="N34" s="30">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
@@ -1773,16 +1913,16 @@
       <c r="B38" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="28">
+      <c r="H38" s="27">
         <v>3.1147079000000002E-16</v>
       </c>
-      <c r="I38" s="28">
+      <c r="I38" s="27">
         <v>0.75869335999999998</v>
       </c>
-      <c r="L38" s="28">
-        <v>0</v>
-      </c>
-      <c r="M38" s="28">
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
         <v>0.75869335999999998</v>
       </c>
       <c r="N38" s="14"/>
@@ -1791,16 +1931,16 @@
       <c r="B39" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="28">
+      <c r="H39" s="27">
         <v>1.3277133999999999</v>
       </c>
-      <c r="I39" s="28">
+      <c r="I39" s="27">
         <v>0.25289779000000001</v>
       </c>
-      <c r="L39" s="28">
+      <c r="L39" s="27">
         <v>1.3277133999999999</v>
       </c>
-      <c r="M39" s="28">
+      <c r="M39" s="27">
         <v>0.25289779000000001</v>
       </c>
     </row>
@@ -1808,16 +1948,16 @@
       <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="H40" s="28">
+      <c r="H40" s="27">
         <v>0.77976818000000003</v>
       </c>
-      <c r="I40" s="28">
+      <c r="I40" s="27">
         <v>0.25289779000000001</v>
       </c>
-      <c r="L40" s="28">
+      <c r="L40" s="27">
         <v>0.77976818000000003</v>
       </c>
-      <c r="M40" s="28">
+      <c r="M40" s="27">
         <v>0.25289779000000001</v>
       </c>
       <c r="AW40" s="2"/>
@@ -1840,16 +1980,16 @@
       <c r="B42" t="s">
         <v>30</v>
       </c>
-      <c r="H42" s="28">
-        <v>0</v>
-      </c>
-      <c r="I42" s="28">
+      <c r="H42" s="27">
+        <v>0</v>
+      </c>
+      <c r="I42" s="27">
         <v>1.1380399999999999</v>
       </c>
-      <c r="L42" s="28">
-        <v>0</v>
-      </c>
-      <c r="M42" s="28">
+      <c r="L42" s="27">
+        <v>0</v>
+      </c>
+      <c r="M42" s="27">
         <v>1.1380399999999999</v>
       </c>
       <c r="N42" s="14"/>
@@ -1858,16 +1998,16 @@
       <c r="B43" t="s">
         <v>31</v>
       </c>
-      <c r="H43" s="28">
+      <c r="H43" s="27">
         <v>1.9915700999999999</v>
       </c>
-      <c r="I43" s="28">
+      <c r="I43" s="27">
         <v>0.37934667999999999</v>
       </c>
-      <c r="L43" s="28">
+      <c r="L43" s="27">
         <v>1.9915700999999999</v>
       </c>
-      <c r="M43" s="28">
+      <c r="M43" s="27">
         <v>0.37934667999999999</v>
       </c>
     </row>
@@ -1875,16 +2015,16 @@
       <c r="B44" t="s">
         <v>32</v>
       </c>
-      <c r="H44" s="28">
+      <c r="H44" s="27">
         <v>1.1696523000000001</v>
       </c>
-      <c r="I44" s="28">
+      <c r="I44" s="27">
         <v>0.37934667999999999</v>
       </c>
-      <c r="L44" s="28">
+      <c r="L44" s="27">
         <v>1.1696523000000001</v>
       </c>
-      <c r="M44" s="28">
+      <c r="M44" s="27">
         <v>0.37934667999999999</v>
       </c>
     </row>
@@ -1942,12 +2082,12 @@
         <v>346.15384999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L50" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -1962,7 +2102,7 @@
         <v>0.75869335800000004</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>31</v>
       </c>
@@ -1973,7 +2113,7 @@
         <v>0.75869335800000004</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>32</v>
       </c>
@@ -1983,18 +2123,9 @@
       <c r="M53" s="1">
         <v>0.75869335800000004</v>
       </c>
-      <c r="AW53" s="25"/>
-      <c r="AX53" s="25"/>
-      <c r="AY53" s="25"/>
-      <c r="AZ53" s="25"/>
-    </row>
-    <row r="54" spans="1:52" s="25" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AW54"/>
-      <c r="AX54"/>
-      <c r="AY54"/>
-      <c r="AZ54"/>
-    </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -2008,9 +2139,9 @@
       <c r="M55" s="1">
         <v>1.1380400369999999</v>
       </c>
-      <c r="N55" s="31"/>
-    </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="N55" s="29"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>31</v>
       </c>
@@ -2021,7 +2152,7 @@
         <v>1.1380400369999999</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>32</v>
       </c>
@@ -2035,29 +2166,29 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>10</v>
       </c>
-      <c r="N58" s="30" cm="1">
+      <c r="N58" s="28" cm="1">
         <f t="array" ref="N58:N59">N23:N24*N77:N78*Q13*S13</f>
         <v>329.67032504999997</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
-      <c r="N59" s="30">
+      <c r="N59" s="28">
         <v>346.15384184999994</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L61" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2203,7 @@
         <v>0.25289778599999996</v>
       </c>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>31</v>
       </c>
@@ -2083,7 +2214,7 @@
         <v>0.25289778599999996</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>32</v>
       </c>
@@ -2093,18 +2224,9 @@
       <c r="M64" s="1">
         <v>0.25289778599999996</v>
       </c>
-      <c r="AW64" s="25"/>
-      <c r="AX64" s="25"/>
-      <c r="AY64" s="25"/>
-      <c r="AZ64" s="25"/>
-    </row>
-    <row r="65" spans="1:52" s="25" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AW65"/>
-      <c r="AX65"/>
-      <c r="AY65"/>
-      <c r="AZ65"/>
-    </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:17" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -2119,7 +2241,7 @@
         <v>0.37934667899999996</v>
       </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>31</v>
       </c>
@@ -2130,7 +2252,7 @@
         <v>0.37934667899999996</v>
       </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>32</v>
       </c>
@@ -2144,18 +2266,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="N69" s="30" cm="1">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N69" s="28" cm="1">
         <f t="array" ref="N69:N70">N29:N30*N77:N78*Q13*S13</f>
         <v>230.76922753499997</v>
       </c>
     </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="N70" s="30">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N70" s="28">
         <v>242.30768929499993</v>
       </c>
     </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L72" s="11" t="s">
         <v>13</v>
       </c>
@@ -2163,17 +2285,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
-      <c r="L73" s="26">
+      <c r="L73" s="25">
         <v>6.6385668999999998</v>
       </c>
-      <c r="M73" s="26">
+      <c r="M73" s="25">
         <v>0.84299261999999997</v>
       </c>
-      <c r="N73" s="26">
+      <c r="N73" s="25">
         <v>0.30106878999999998</v>
       </c>
       <c r="P73" s="1">
@@ -2183,17 +2305,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
-      <c r="L74" s="26">
-        <v>0</v>
-      </c>
-      <c r="M74" s="26">
+      <c r="L74" s="25">
+        <v>0</v>
+      </c>
+      <c r="M74" s="25">
         <v>0.42149630999999999</v>
       </c>
-      <c r="N74" s="26">
+      <c r="N74" s="25">
         <v>1.505344E-2</v>
       </c>
       <c r="P74" s="1">
@@ -2203,41 +2325,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L76" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
-      <c r="L77" s="27" cm="1">
+      <c r="L77" s="26" cm="1">
         <f t="array" ref="L77:N78">MMULT(P73:Q74,L73:N74)</f>
         <v>6.6385668999999998</v>
       </c>
-      <c r="M77" s="27">
+      <c r="M77" s="26">
         <v>0.84299261999999997</v>
       </c>
-      <c r="N77" s="27">
+      <c r="N77" s="26">
         <v>0.30106878999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>11</v>
       </c>
-      <c r="L78" s="27">
+      <c r="L78" s="26">
         <v>6.6385668999999998</v>
       </c>
-      <c r="M78" s="27">
+      <c r="M78" s="26">
         <v>1.26448893</v>
       </c>
-      <c r="N78" s="27">
+      <c r="N78" s="26">
         <v>0.31612222999999995</v>
       </c>
     </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L80" s="11" t="s">
         <v>20</v>
       </c>
@@ -2371,6 +2493,963 @@
         <v>346.15384499999999</v>
       </c>
       <c r="N92" s="17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044E5F7A-12EA-4F3D-841B-2D3ACD841AA6}">
+  <dimension ref="A1:AD52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="6" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="S41" sqref="S41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="17" max="21" width="4.7109375" customWidth="1"/>
+    <col min="22" max="22" width="3" customWidth="1"/>
+    <col min="23" max="23" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="30" width="5.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="H7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="17" cm="1">
+        <f t="array" ref="Q8:U8">MMULT(H8:I8,TRANSPOSE(H34:I38))</f>
+        <v>1.5</v>
+      </c>
+      <c r="R8" s="17">
+        <v>2</v>
+      </c>
+      <c r="S8" s="17">
+        <v>4</v>
+      </c>
+      <c r="T8" s="17">
+        <v>1</v>
+      </c>
+      <c r="U8" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="Z8" s="19" cm="1">
+        <f t="array" ref="Z8:AD8">_xlfn.ANCHORARRAY(Q8)-_xlfn.ANCHORARRAY(Q10)-_xlfn.ANCHORARRAY(Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="H9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="17" cm="1">
+        <f t="array" ref="Q10:U10">MMULT(K8:M8,TRANSPOSE(K34:M38))</f>
+        <v>0.5</v>
+      </c>
+      <c r="R10" s="17">
+        <v>0</v>
+      </c>
+      <c r="S10" s="17">
+        <v>1</v>
+      </c>
+      <c r="T10" s="17">
+        <v>-1</v>
+      </c>
+      <c r="U10" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="Z10" s="32" cm="1">
+        <f t="array" ref="Z10:AD11">TRANSPOSE(K34:L38)-MMULT(H10:I11,TRANSPOSE(H34:I38))</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z11" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="36">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1" cm="1">
+        <f t="array" ref="Q12:U12">O8*TRANSPOSE(O19:O23)</f>
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>2</v>
+      </c>
+      <c r="S12" s="1">
+        <v>3</v>
+      </c>
+      <c r="T12" s="1">
+        <v>2</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="12" cm="1">
+        <f t="array" ref="O13">SUM(MMULT(K34:M38,K25:M25*_xlfn.MUNIT(3)))</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>1</v>
+      </c>
+      <c r="T22" s="1">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
+        <v>1</v>
+      </c>
+      <c r="T23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O26" s="40">
+        <f>M26*M30</f>
+        <v>1</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J27" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="O27" s="40">
+        <f>M27*M30</f>
+        <v>9</v>
+      </c>
+      <c r="P27" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J28" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="O28" s="40">
+        <f>M30*M28</f>
+        <v>4</v>
+      </c>
+      <c r="P28" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J29" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O29" s="40">
+        <f>M30*M29</f>
+        <v>6</v>
+      </c>
+      <c r="P29" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K30" s="1">
+        <v>10</v>
+      </c>
+      <c r="L30" s="1">
+        <v>10</v>
+      </c>
+      <c r="M30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J31" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="I34" s="38">
+        <v>1</v>
+      </c>
+      <c r="K34" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L34" s="38">
+        <v>1</v>
+      </c>
+      <c r="M34" s="38">
+        <v>-0.5</v>
+      </c>
+      <c r="O34" s="17">
+        <f>ABS(M34)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" s="38">
+        <v>0</v>
+      </c>
+      <c r="I35" s="38">
+        <v>2</v>
+      </c>
+      <c r="K35" s="38">
+        <v>0</v>
+      </c>
+      <c r="L35" s="38">
+        <v>2</v>
+      </c>
+      <c r="M35" s="38">
+        <v>0</v>
+      </c>
+      <c r="O35" s="17">
+        <f t="shared" ref="O35:O38" si="0">ABS(M35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="38">
+        <v>2</v>
+      </c>
+      <c r="I36" s="38">
+        <v>2</v>
+      </c>
+      <c r="K36" s="38">
+        <v>2</v>
+      </c>
+      <c r="L36" s="38">
+        <v>2</v>
+      </c>
+      <c r="M36" s="38">
+        <v>-1</v>
+      </c>
+      <c r="O36" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L37" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="M37" s="38">
+        <v>1</v>
+      </c>
+      <c r="O37" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="I38" s="38">
+        <v>0</v>
+      </c>
+      <c r="K38" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="L38" s="38">
+        <v>0</v>
+      </c>
+      <c r="M38" s="38">
+        <v>-1.5</v>
+      </c>
+      <c r="O38" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L40" s="10"/>
+      <c r="M40" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="40" cm="1">
+        <f t="array" ref="K41:L45">K30:L30*K13:L17</f>
+        <v>10</v>
+      </c>
+      <c r="L41" s="41">
+        <v>2</v>
+      </c>
+      <c r="M41" s="40" cm="1">
+        <f t="array" ref="M41:M45">O28-MMULT(Q19:U23,M34:M38)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="K42" s="40">
+        <v>10</v>
+      </c>
+      <c r="L42" s="41">
+        <v>5</v>
+      </c>
+      <c r="M42" s="40">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K43" s="40">
+        <v>10</v>
+      </c>
+      <c r="L43" s="41">
+        <v>4</v>
+      </c>
+      <c r="M43" s="40">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" s="40">
+        <v>10</v>
+      </c>
+      <c r="L44" s="41">
+        <v>1</v>
+      </c>
+      <c r="M44" s="40">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="K45" s="40">
+        <v>10</v>
+      </c>
+      <c r="L45" s="41">
+        <v>0</v>
+      </c>
+      <c r="M45" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L46" s="10"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K47" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="K48" s="31" cm="1">
+        <f t="array" ref="K48:L52">K30:L30*K19:L23</f>
+        <v>0</v>
+      </c>
+      <c r="L48" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="K49" s="31">
+        <v>0</v>
+      </c>
+      <c r="L49" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="K50" s="31">
+        <v>0</v>
+      </c>
+      <c r="L50" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="K51" s="31">
+        <v>0</v>
+      </c>
+      <c r="L51" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="K52" s="31">
+        <v>0</v>
+      </c>
+      <c r="L52" s="31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
storage model with and without v2g working in Excel
</commit_message>
<xml_diff>
--- a/default/4_sut_multi_year_hourly/concept.xlsx
+++ b/default/4_sut_multi_year_hourly/concept.xlsx
@@ -8,38 +8,63 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\4_sut_multi_year_hourly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1598FEAA-1538-40CB-918A-D8A09445639B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1F5BC8-B78A-46A4-8434-D52059DBC2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
   </bookViews>
   <sheets>
     <sheet name="hours" sheetId="6" r:id="rId1"/>
     <sheet name="storage" sheetId="11" r:id="rId2"/>
+    <sheet name="storage_bev" sheetId="13" r:id="rId3"/>
+    <sheet name="storage_bev_v2g" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="3" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="3" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="3" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">hours!$H$38:$I$40,hours!$H$42:$I$44,hours!$L$38:$M$40,hours!$L$42:$M$44,hours!$L$47:$N$48,hours!$H$47:$J$48,hours!$L$73:$N$74</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">storage!$H$34:$I$38,storage!$K$34:$M$38</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">storage!$H$35:$I$39,storage!$K$35:$M$39</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">storage_bev!$H$40:$K$44,storage_bev!$M$40:$Q$44</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">storage_bev_v2g!$H$40:$K$44,storage_bev_v2g!$M$40:$Q$44</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">hours!$AM$9:$AN$10</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">storage!$Z$8:$AD$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">storage_bev!$AG$9:$AK$11</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">storage_bev_v2g!$AG$9:$AK$11</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
-    <definedName name="solver_lhs10" localSheetId="1" hidden="1">storage!$O$34:$O$38</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">storage!$M$35:$M$39</definedName>
+    <definedName name="solver_lhs10" localSheetId="2" hidden="1">storage_bev!$Q$40:$Q$44</definedName>
+    <definedName name="solver_lhs10" localSheetId="3" hidden="1">storage_bev_v2g!$Q$40:$Q$44</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">hours!$N$47:$N$48</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">storage!$M$35:$M$39</definedName>
     <definedName name="solver_lhs12" localSheetId="0" hidden="1">hours!$L$38:$M$40</definedName>
     <definedName name="solver_lhs13" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
     <definedName name="solver_lhs14" localSheetId="0" hidden="1">hours!$N$47:$N$48</definedName>
@@ -49,33 +74,62 @@
     <definedName name="solver_lhs18" localSheetId="0" hidden="1">hours!$L$42:$M$44</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">hours!$AM$14:$AN$16</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">storage!$Z$10:$AD$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">storage_bev!$AG$13:$AK$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">storage_bev_v2g!$AG$13:$AK$16</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">hours!$AP$9:$AR$9</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">storage!$K$34:$L$38</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">storage!$K$35:$L$39</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">storage_bev!$M$40:$O$44</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">storage_bev_v2g!$M$40:$O$44</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">hours!$AT$9:$AV$9</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">storage!$K$34:$L$38</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">storage!$K$35:$L$39</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">storage_bev!$M$40:$O$44</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">storage_bev_v2g!$M$40:$O$44</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">hours!$AP$14:$AR$15</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">storage!$M$42:$M$46</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">storage_bev!$Q$47:$Q$51</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">storage_bev_v2g!$Q$47:$Q$51</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">hours!$AT$14:$AV$15</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">storage!$H$34:$I$38</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">storage!$H$35:$I$39</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">storage_bev!$Q$40:$Q$44</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">storage_bev_v2g!$Q$40:$Q$44</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">hours!$AX$9:$AY$9</definedName>
     <definedName name="solver_lhs7" localSheetId="1" hidden="1">storage!$O$29</definedName>
+    <definedName name="solver_lhs7" localSheetId="2" hidden="1">storage_bev!$Q$40:$Q$44</definedName>
+    <definedName name="solver_lhs7" localSheetId="3" hidden="1">storage_bev_v2g!$Q$40:$Q$44</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">hours!$AX$14:$AY$15</definedName>
-    <definedName name="solver_lhs8" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">storage!$M$42:$M$46</definedName>
+    <definedName name="solver_lhs8" localSheetId="2" hidden="1">storage_bev!$H$40:$K$44</definedName>
+    <definedName name="solver_lhs8" localSheetId="3" hidden="1">storage_bev_v2g!$H$40:$K$44</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">hours!$L$38:$M$40</definedName>
-    <definedName name="solver_lhs9" localSheetId="1" hidden="1">storage!$M$41:$M$45</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">storage!$M$42:$M$46</definedName>
+    <definedName name="solver_lhs9" localSheetId="2" hidden="1">storage_bev!$Q$47:$Q$51</definedName>
+    <definedName name="solver_lhs9" localSheetId="3" hidden="1">storage_bev_v2g!$Q$47:$Q$51</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">14</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">9</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">11</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">10</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">9</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">hours!$Q$17</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">storage!$O$12</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">storage_bev!$S$13</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">storage_bev_v2g!$S$13</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">3</definedName>
@@ -85,25 +139,46 @@
     <definedName name="solver_rel18" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">hours!$L$55:$M$57</definedName>
     <definedName name="solver_rhs10" localSheetId="1" hidden="1">storage!$M$31</definedName>
+    <definedName name="solver_rhs10" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs10" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">hours!$N$58:$N$59</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">storage!$M$32</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">hours!$L$62:$M$64</definedName>
     <definedName name="solver_rhs13" localSheetId="0" hidden="1">hours!$L$66:$M$68</definedName>
     <definedName name="solver_rhs14" localSheetId="0" hidden="1">hours!$N$69:$N$70</definedName>
@@ -113,34 +188,64 @@
     <definedName name="solver_rhs18" localSheetId="0" hidden="1">hours!$L$66:$M$68</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">storage!$K$48:$L$52</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">storage!$K$49:$L$53</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">storage_bev!$M$54:$O$58</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">storage_bev_v2g!$M$54:$O$58</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">storage!$K$41:$L$45</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">storage!$K$42:$L$46</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">storage_bev!$M$47:$O$51</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">storage_bev_v2g!$M$47:$O$51</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">storage!$M$30</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">storage_bev!$S$32</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">storage_bev_v2g!$S$32</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">storage_bev!$Q$36</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">storage_bev_v2g!$Q$36</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs7" localSheetId="1" hidden="1">storage!$M$45</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">storage!$M$46</definedName>
+    <definedName name="solver_rhs7" localSheetId="2" hidden="1">storage_bev!$Q$37</definedName>
+    <definedName name="solver_rhs7" localSheetId="3" hidden="1">storage_bev_v2g!$Q$37</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs8" localSheetId="1" hidden="1">storage!$O$26</definedName>
+    <definedName name="solver_rhs8" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs8" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">hours!$L$51:$M$53</definedName>
     <definedName name="solver_rhs9" localSheetId="1" hidden="1">storage!$O$27</definedName>
+    <definedName name="solver_rhs9" localSheetId="2" hidden="1">storage_bev!$S$31</definedName>
+    <definedName name="solver_rhs9" localSheetId="3" hidden="1">storage_bev_v2g!$S$31</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -163,7 +268,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -185,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="113">
   <si>
     <t>flows</t>
   </si>
@@ -481,16 +586,49 @@
     <t>SOC min</t>
   </si>
   <si>
-    <t>c/d max rate</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
-    <t>c/d</t>
-  </si>
-  <si>
     <t>X_h'-d*Q_h' == 0</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>BEV</t>
+  </si>
+  <si>
+    <t>EE coal</t>
+  </si>
+  <si>
+    <t>t.3 s</t>
+  </si>
+  <si>
+    <t>BEV battery</t>
+  </si>
+  <si>
+    <t>f.1s</t>
+  </si>
+  <si>
+    <t>EE BEV</t>
+  </si>
+  <si>
+    <t>max charge rate</t>
+  </si>
+  <si>
+    <t>max discharge rate</t>
+  </si>
+  <si>
+    <t>X_max</t>
+  </si>
+  <si>
+    <t>X_min</t>
+  </si>
+  <si>
+    <t>t.3 eng</t>
+  </si>
+  <si>
+    <t>BEV engine</t>
   </si>
 </sst>
 </file>
@@ -717,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -764,10 +902,16 @@
     </xf>
     <xf numFmtId="167" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2509,13 +2653,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044E5F7A-12EA-4F3D-841B-2D3ACD841AA6}">
-  <dimension ref="A1:AD52"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="6" topLeftCell="H16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="X17" sqref="X17"/>
+      <selection pane="bottomRight" activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2674,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="43"/>
+    <col min="14" max="14" width="9.140625" style="42"/>
     <col min="17" max="21" width="4.7109375" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
     <col min="23" max="23" width="4.28515625" bestFit="1" customWidth="1"/>
@@ -2629,7 +2773,7 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="M4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O4" t="s">
         <v>29</v>
@@ -2716,20 +2860,20 @@
         <v>10</v>
       </c>
       <c r="Q8" s="17" cm="1">
-        <f t="array" ref="Q8:U8">MMULT(H8:I8,TRANSPOSE(H34:I38))</f>
-        <v>0</v>
+        <f t="array" ref="Q8:U8">MMULT(H8:I8,TRANSPOSE(H35:I39))</f>
+        <v>3</v>
       </c>
       <c r="R8" s="17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S8" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T8" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="19" cm="1">
         <f t="array" ref="Z8:AD8">_xlfn.ANCHORARRAY(Q8)-_xlfn.ANCHORARRAY(Q10)-_xlfn.ANCHORARRAY(Q12)</f>
@@ -2756,7 +2900,7 @@
         <v>90</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -2776,23 +2920,23 @@
         <v>0</v>
       </c>
       <c r="Q10" s="17" cm="1">
-        <f t="array" ref="Q10:U10">MMULT(K8:M8,TRANSPOSE(K34:M38))</f>
+        <f t="array" ref="Q10:U10">MMULT(K8:M8,TRANSPOSE(K35:M39))</f>
+        <v>2</v>
+      </c>
+      <c r="R10" s="17">
+        <v>3</v>
+      </c>
+      <c r="S10" s="17">
+        <v>0</v>
+      </c>
+      <c r="T10" s="17">
         <v>-1</v>
       </c>
-      <c r="R10" s="17">
-        <v>6</v>
-      </c>
-      <c r="S10" s="17">
-        <v>-3</v>
-      </c>
-      <c r="T10" s="17">
+      <c r="U10" s="17">
         <v>-2</v>
       </c>
-      <c r="U10" s="17">
-        <v>2</v>
-      </c>
       <c r="Z10" s="32" cm="1">
-        <f t="array" ref="Z10:AD11">TRANSPOSE(K34:L38)-MMULT(H10:I11,TRANSPOSE(H34:I38))</f>
+        <f t="array" ref="Z10:AD11">TRANSPOSE(K35:L39)-MMULT(H10:I11,TRANSPOSE(H35:I39))</f>
         <v>0</v>
       </c>
       <c r="AA10" s="33">
@@ -2824,9 +2968,6 @@
       <c r="I11" s="1">
         <v>1</v>
       </c>
-      <c r="Q11" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="Z11" s="35">
         <v>0</v>
       </c>
@@ -2848,23 +2989,23 @@
         <v>17</v>
       </c>
       <c r="O12" s="12" cm="1">
-        <f t="array" ref="O12">SUM(MMULT(K34:M38,K25:M25*_xlfn.MUNIT(3)))</f>
+        <f t="array" ref="O12">SUM(MMULT(K35:M39,K25:M25*_xlfn.MUNIT(3)))</f>
         <v>12</v>
       </c>
-      <c r="Q12" s="1" cm="1">
+      <c r="Q12" s="16" cm="1">
         <f t="array" ref="Q12:U12">O8*TRANSPOSE(O19:O23)</f>
         <v>1</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="16">
         <v>2</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="16">
         <v>3</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="16">
         <v>2</v>
       </c>
-      <c r="U12" s="1">
+      <c r="U12" s="16">
         <v>2</v>
       </c>
     </row>
@@ -3178,188 +3319,159 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="J31" s="13" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="M31" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J32" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="M32" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H33" s="11" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H34" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K34" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="O33" s="42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="38">
-        <v>0</v>
-      </c>
-      <c r="I34" s="38">
-        <v>0</v>
-      </c>
-      <c r="K34" s="38">
-        <v>0</v>
-      </c>
-      <c r="L34" s="38">
-        <v>0</v>
-      </c>
-      <c r="M34" s="38">
-        <v>1</v>
-      </c>
-      <c r="O34" s="17">
-        <f>ABS(M34)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="H35" s="38">
+        <v>0</v>
+      </c>
+      <c r="I35" s="38">
+        <v>3</v>
+      </c>
+      <c r="K35" s="38">
+        <v>0</v>
+      </c>
+      <c r="L35" s="38">
+        <v>3</v>
+      </c>
+      <c r="M35" s="38">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="38">
-        <v>0</v>
-      </c>
-      <c r="I35" s="38">
-        <v>8</v>
-      </c>
-      <c r="K35" s="38">
-        <v>0</v>
-      </c>
-      <c r="L35" s="38">
-        <v>8</v>
-      </c>
-      <c r="M35" s="38">
-        <v>-6</v>
-      </c>
-      <c r="O35" s="17">
-        <f t="shared" ref="O35:O38" si="0">ABS(M35)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="H36" s="38">
+        <v>0</v>
+      </c>
+      <c r="I36" s="38">
+        <v>5</v>
+      </c>
+      <c r="K36" s="38">
+        <v>0</v>
+      </c>
+      <c r="L36" s="38">
+        <v>5</v>
+      </c>
+      <c r="M36" s="38">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="38">
-        <v>0</v>
-      </c>
-      <c r="I36" s="38">
-        <v>0</v>
-      </c>
-      <c r="K36" s="38">
-        <v>0</v>
-      </c>
-      <c r="L36" s="38">
-        <v>0</v>
-      </c>
-      <c r="M36" s="38">
+      <c r="H37" s="38">
+        <v>0</v>
+      </c>
+      <c r="I37" s="38">
         <v>3</v>
       </c>
-      <c r="O36" s="17">
-        <f t="shared" si="0"/>
+      <c r="K37" s="38">
+        <v>0</v>
+      </c>
+      <c r="L37" s="38">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="M37" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-      <c r="H37" s="38">
-        <v>0</v>
-      </c>
-      <c r="I37" s="38">
-        <v>0</v>
-      </c>
-      <c r="K37" s="38">
-        <v>0</v>
-      </c>
-      <c r="L37" s="38">
-        <v>0</v>
-      </c>
-      <c r="M37" s="38">
+      <c r="H38" s="38">
+        <v>0</v>
+      </c>
+      <c r="I38" s="38">
+        <v>1</v>
+      </c>
+      <c r="K38" s="38">
+        <v>0</v>
+      </c>
+      <c r="L38" s="38">
+        <v>1</v>
+      </c>
+      <c r="M38" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="38">
+        <v>0</v>
+      </c>
+      <c r="I39" s="38">
+        <v>0</v>
+      </c>
+      <c r="K39" s="38">
+        <v>0</v>
+      </c>
+      <c r="L39" s="38">
+        <v>0</v>
+      </c>
+      <c r="M39" s="38">
         <v>2</v>
       </c>
-      <c r="O37" s="17">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="38">
-        <v>0</v>
-      </c>
-      <c r="I38" s="38">
-        <v>4</v>
-      </c>
-      <c r="K38" s="38">
-        <v>0</v>
-      </c>
-      <c r="L38" s="38">
-        <v>4</v>
-      </c>
-      <c r="M38" s="38">
-        <v>-2</v>
-      </c>
-      <c r="O38" s="17">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K40" s="11" t="s">
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="11" t="s">
+      <c r="L41" s="10"/>
+      <c r="M41" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>30</v>
       </c>
-      <c r="K41" s="40" cm="1">
-        <f t="array" ref="K41:L45">K30:L30*K13:L17</f>
-        <v>10</v>
-      </c>
-      <c r="L41" s="41">
-        <v>10</v>
-      </c>
-      <c r="M41" s="40" cm="1">
-        <f t="array" ref="M41:M45">O28-MMULT(Q19:U23,M34:M38)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="K42" s="40">
+      <c r="K42" s="40" cm="1">
+        <f t="array" ref="K42:L46">K30:L30*K13:L17</f>
         <v>10</v>
       </c>
       <c r="L42" s="41">
         <v>10</v>
       </c>
-      <c r="M42" s="40">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M42" s="40" cm="1">
+        <f t="array" ref="M42:M46">O28-MMULT(Q19:U23,M35:M39)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K43" s="40">
         <v>10</v>
@@ -3368,12 +3480,12 @@
         <v>10</v>
       </c>
       <c r="M43" s="40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="K44" s="40">
         <v>10</v>
@@ -3382,12 +3494,12 @@
         <v>10</v>
       </c>
       <c r="M44" s="40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K45" s="40">
         <v>10</v>
@@ -3396,34 +3508,37 @@
         <v>10</v>
       </c>
       <c r="M45" s="40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="K46" s="40">
+        <v>10</v>
+      </c>
+      <c r="L46" s="41">
+        <v>10</v>
+      </c>
+      <c r="M46" s="40">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L46" s="10"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K47" s="11" t="s">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L47" s="10"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K48" s="11" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="K48" s="31" cm="1">
-        <f t="array" ref="K48:L52">K30:L30*K19:L23</f>
-        <v>0</v>
-      </c>
-      <c r="L48" s="31">
-        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>31</v>
-      </c>
-      <c r="K49" s="31">
+        <v>30</v>
+      </c>
+      <c r="K49" s="31" cm="1">
+        <f t="array" ref="K49:L53">K30:L30*K19:L23</f>
         <v>0</v>
       </c>
       <c r="L49" s="31">
@@ -3432,7 +3547,7 @@
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K50" s="31">
         <v>0</v>
@@ -3443,7 +3558,7 @@
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="K51" s="31">
         <v>0</v>
@@ -3454,12 +3569,3017 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="K52" s="31">
+        <v>0</v>
+      </c>
+      <c r="L52" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>79</v>
       </c>
-      <c r="K52" s="31">
-        <v>0</v>
-      </c>
-      <c r="L52" s="31">
+      <c r="K53" s="31">
+        <v>0</v>
+      </c>
+      <c r="L53" s="31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65AABF1-D5A8-4799-AA08-57874A1B0E10}">
+  <dimension ref="A1:AK58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="7" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="M44" sqref="M44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="17" width="6.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" customWidth="1"/>
+    <col min="21" max="37" width="6" customWidth="1"/>
+    <col min="38" max="39" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>104</v>
+      </c>
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG8" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>-1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>10</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA9" s="17" cm="1">
+        <f t="array" ref="AA9:AE11">MMULT(H9:K11,TRANSPOSE(H40:K44))</f>
+        <v>1</v>
+      </c>
+      <c r="AB9" s="17">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="17">
+        <v>6</v>
+      </c>
+      <c r="AD9" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="17">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="3" cm="1">
+        <f t="array" ref="AG9:AK11">AA9:AE11-AA13:AE15-AA17:AE19</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="47">
+        <v>1.2</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>0</v>
+      </c>
+      <c r="S10" s="16">
+        <v>0</v>
+      </c>
+      <c r="U10" s="16">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16">
+        <v>0</v>
+      </c>
+      <c r="W10" s="16">
+        <v>0</v>
+      </c>
+      <c r="X10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="17">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>10</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="17">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG12" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="12" cm="1">
+        <f t="array" ref="S13">SUM(MMULT(M40:O44,M30:O30*_xlfn.MUNIT(3)))</f>
+        <v>31</v>
+      </c>
+      <c r="AA13" s="17" cm="1">
+        <f t="array" ref="AA13:AE15">MMULT(M9:Q11,TRANSPOSE(M40:Q44))</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="17">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3" cm="1">
+        <f t="array" ref="AG13:AK16">TRANSPOSE(M40:P44)-MMULT(H13:K16,TRANSPOSE(H40:K44))</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="17">
+        <v>6</v>
+      </c>
+      <c r="AC14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA17" s="16" cm="1">
+        <f t="array" ref="AA17:AE19">S9:S11*U9:Y11</f>
+        <v>1</v>
+      </c>
+      <c r="AB17" s="16">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="16">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="16">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>5</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="16">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="42"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="42"/>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="S23" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA23" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA29" s="42"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="1">
+        <v>3</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="42"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="S31" s="40">
+        <f>Q31*Q35</f>
+        <v>1</v>
+      </c>
+      <c r="T31" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="42"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="L32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="S32" s="40">
+        <f>Q32*Q35</f>
+        <v>20</v>
+      </c>
+      <c r="T32" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="42"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="S33" s="40">
+        <f>Q35*Q33</f>
+        <v>8</v>
+      </c>
+      <c r="T33" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="39"/>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="42"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L34" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="42"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L35" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="1">
+        <v>20</v>
+      </c>
+      <c r="N35" s="1">
+        <v>20</v>
+      </c>
+      <c r="O35" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA35" s="42"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>-3</v>
+      </c>
+      <c r="AA36" s="42"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L37" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="H39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="18">
+        <v>1</v>
+      </c>
+      <c r="I40" s="18">
+        <v>0</v>
+      </c>
+      <c r="J40" s="18">
+        <v>0</v>
+      </c>
+      <c r="K40" s="18">
+        <v>0</v>
+      </c>
+      <c r="M40" s="18">
+        <v>1</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0</v>
+      </c>
+      <c r="O40" s="18">
+        <v>0</v>
+      </c>
+      <c r="P40" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="18">
+        <v>0</v>
+      </c>
+      <c r="I41" s="18">
+        <v>4</v>
+      </c>
+      <c r="J41" s="18">
+        <v>6</v>
+      </c>
+      <c r="K41" s="18">
+        <v>5</v>
+      </c>
+      <c r="M41" s="18">
+        <v>0</v>
+      </c>
+      <c r="N41" s="18">
+        <v>4</v>
+      </c>
+      <c r="O41" s="18">
+        <v>5</v>
+      </c>
+      <c r="P41" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="18">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="18">
+        <v>0</v>
+      </c>
+      <c r="I42" s="18">
+        <v>6</v>
+      </c>
+      <c r="J42" s="18">
+        <v>0</v>
+      </c>
+      <c r="K42" s="18">
+        <v>0</v>
+      </c>
+      <c r="M42" s="18">
+        <v>0</v>
+      </c>
+      <c r="N42" s="18">
+        <v>6</v>
+      </c>
+      <c r="O42" s="18">
+        <v>0</v>
+      </c>
+      <c r="P42" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="18">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="18">
+        <v>0</v>
+      </c>
+      <c r="I43" s="18">
+        <v>2</v>
+      </c>
+      <c r="J43" s="18">
+        <v>6</v>
+      </c>
+      <c r="K43" s="18">
+        <v>5</v>
+      </c>
+      <c r="M43" s="18">
+        <v>0</v>
+      </c>
+      <c r="N43" s="18">
+        <v>2</v>
+      </c>
+      <c r="O43" s="18">
+        <v>5</v>
+      </c>
+      <c r="P43" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q43" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="18">
+        <v>2</v>
+      </c>
+      <c r="I44" s="18">
+        <v>0</v>
+      </c>
+      <c r="J44" s="18">
+        <v>0</v>
+      </c>
+      <c r="K44" s="18">
+        <v>0</v>
+      </c>
+      <c r="M44" s="18">
+        <v>2</v>
+      </c>
+      <c r="N44" s="18">
+        <v>0</v>
+      </c>
+      <c r="O44" s="18">
+        <v>0</v>
+      </c>
+      <c r="P44" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="M46" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" s="45"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="17" cm="1">
+        <f t="array" ref="M47:O51">M18:O22*M35:O35</f>
+        <v>18</v>
+      </c>
+      <c r="N47" s="17">
+        <v>0</v>
+      </c>
+      <c r="O47" s="46">
+        <v>20</v>
+      </c>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="43" cm="1">
+        <f t="array" ref="Q47:Q51">S33-MMULT(AA24:AE28,P40:P44+Q40:Q44)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M48" s="17">
+        <v>18</v>
+      </c>
+      <c r="N48" s="17">
+        <v>4</v>
+      </c>
+      <c r="O48" s="46">
+        <v>20</v>
+      </c>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="17">
+        <v>18</v>
+      </c>
+      <c r="N49" s="17">
+        <v>10</v>
+      </c>
+      <c r="O49" s="46">
+        <v>20</v>
+      </c>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="M50" s="17">
+        <v>18</v>
+      </c>
+      <c r="N50" s="17">
+        <v>6</v>
+      </c>
+      <c r="O50" s="46">
+        <v>20</v>
+      </c>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="M51" s="17">
+        <v>18</v>
+      </c>
+      <c r="N51" s="17">
+        <v>0</v>
+      </c>
+      <c r="O51" s="46">
+        <v>20</v>
+      </c>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O52" s="45"/>
+      <c r="P52" s="10"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M53" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" s="17" cm="1">
+        <f t="array" ref="M54:O58">M24:O28*M35:O35</f>
+        <v>0</v>
+      </c>
+      <c r="N54" s="17">
+        <v>0</v>
+      </c>
+      <c r="O54" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="M55" s="17">
+        <v>0</v>
+      </c>
+      <c r="N55" s="17">
+        <v>0</v>
+      </c>
+      <c r="O55" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="M56" s="17">
+        <v>0</v>
+      </c>
+      <c r="N56" s="17">
+        <v>0</v>
+      </c>
+      <c r="O56" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="M57" s="17">
+        <v>0</v>
+      </c>
+      <c r="N57" s="17">
+        <v>0</v>
+      </c>
+      <c r="O57" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="M58" s="17">
+        <v>0</v>
+      </c>
+      <c r="N58" s="17">
+        <v>0</v>
+      </c>
+      <c r="O58" s="17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CFFDF8-75E4-4E24-B37F-4C7F08B91489}">
+  <dimension ref="A1:AK58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="Y38" sqref="Y38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="17" width="6.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" customWidth="1"/>
+    <col min="21" max="37" width="6" customWidth="1"/>
+    <col min="38" max="39" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>104</v>
+      </c>
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG8" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>-1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>10</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA9" s="17" cm="1">
+        <f t="array" ref="AA9:AE11">MMULT(H9:K11,TRANSPOSE(H40:K44))</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="17">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="17">
+        <v>6</v>
+      </c>
+      <c r="AD9" s="17">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3" cm="1">
+        <f t="array" ref="AG9:AK11">AA9:AE11-AA13:AE15-AA17:AE19</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="47">
+        <v>1.2</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>0</v>
+      </c>
+      <c r="S10" s="16">
+        <v>0</v>
+      </c>
+      <c r="U10" s="16">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16">
+        <v>0</v>
+      </c>
+      <c r="W10" s="16">
+        <v>0</v>
+      </c>
+      <c r="X10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="17">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>10</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="17">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG12" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="12" cm="1">
+        <f t="array" ref="S13">SUM(MMULT(M40:O44,M30:O30*_xlfn.MUNIT(3)))</f>
+        <v>25</v>
+      </c>
+      <c r="AA13" s="17" cm="1">
+        <f t="array" ref="AA13:AE15">MMULT(M9:Q11,TRANSPOSE(M40:Q44))</f>
+        <v>-1</v>
+      </c>
+      <c r="AB13" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="17">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="17">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="17">
+        <v>-2</v>
+      </c>
+      <c r="AG13" s="3" cm="1">
+        <f t="array" ref="AG13:AK16">TRANSPOSE(M40:P44)-MMULT(H13:K16,TRANSPOSE(H40:K44))</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="17">
+        <v>6</v>
+      </c>
+      <c r="AC14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA17" s="16" cm="1">
+        <f t="array" ref="AA17:AE19">S9:S11*U9:Y11</f>
+        <v>1</v>
+      </c>
+      <c r="AB17" s="16">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="16">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="16">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>5</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="16">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="42"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="42"/>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="S23" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA23" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA29" s="42"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="1">
+        <v>3</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="42"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="S31" s="40">
+        <f>Q31*Q35</f>
+        <v>1</v>
+      </c>
+      <c r="T31" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="42"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="L32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="S32" s="40">
+        <f>Q32*Q35</f>
+        <v>20</v>
+      </c>
+      <c r="T32" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="42"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="S33" s="40">
+        <f>Q35*Q33</f>
+        <v>8</v>
+      </c>
+      <c r="T33" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="39"/>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="42"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L34" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="42"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L35" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="1">
+        <v>20</v>
+      </c>
+      <c r="N35" s="1">
+        <v>20</v>
+      </c>
+      <c r="O35" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA35" s="42"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>-3</v>
+      </c>
+      <c r="AA36" s="42"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L37" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="H39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="18">
+        <v>0</v>
+      </c>
+      <c r="I40" s="18">
+        <v>0</v>
+      </c>
+      <c r="J40" s="18">
+        <v>0</v>
+      </c>
+      <c r="K40" s="18">
+        <v>0</v>
+      </c>
+      <c r="M40" s="18">
+        <v>0</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0</v>
+      </c>
+      <c r="O40" s="18">
+        <v>0</v>
+      </c>
+      <c r="P40" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="18">
+        <v>0</v>
+      </c>
+      <c r="I41" s="18">
+        <v>4</v>
+      </c>
+      <c r="J41" s="18">
+        <v>6</v>
+      </c>
+      <c r="K41" s="18">
+        <v>5</v>
+      </c>
+      <c r="M41" s="18">
+        <v>0</v>
+      </c>
+      <c r="N41" s="18">
+        <v>4</v>
+      </c>
+      <c r="O41" s="18">
+        <v>5</v>
+      </c>
+      <c r="P41" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="18">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="18">
+        <v>0</v>
+      </c>
+      <c r="I42" s="18">
+        <v>6</v>
+      </c>
+      <c r="J42" s="18">
+        <v>0</v>
+      </c>
+      <c r="K42" s="18">
+        <v>0</v>
+      </c>
+      <c r="M42" s="18">
+        <v>0</v>
+      </c>
+      <c r="N42" s="18">
+        <v>6</v>
+      </c>
+      <c r="O42" s="18">
+        <v>0</v>
+      </c>
+      <c r="P42" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="18">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="18">
+        <v>0</v>
+      </c>
+      <c r="I43" s="18">
+        <v>5</v>
+      </c>
+      <c r="J43" s="18">
+        <v>6</v>
+      </c>
+      <c r="K43" s="18">
+        <v>5</v>
+      </c>
+      <c r="M43" s="18">
+        <v>0</v>
+      </c>
+      <c r="N43" s="18">
+        <v>5</v>
+      </c>
+      <c r="O43" s="18">
+        <v>5</v>
+      </c>
+      <c r="P43" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q43" s="18">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="18">
+        <v>0</v>
+      </c>
+      <c r="I44" s="18">
+        <v>0</v>
+      </c>
+      <c r="J44" s="18">
+        <v>0</v>
+      </c>
+      <c r="K44" s="18">
+        <v>0</v>
+      </c>
+      <c r="M44" s="18">
+        <v>0</v>
+      </c>
+      <c r="N44" s="18">
+        <v>0</v>
+      </c>
+      <c r="O44" s="18">
+        <v>0</v>
+      </c>
+      <c r="P44" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="M46" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" s="45"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="17" cm="1">
+        <f t="array" ref="M47:O51">M18:O22*M35:O35</f>
+        <v>18</v>
+      </c>
+      <c r="N47" s="17">
+        <v>0</v>
+      </c>
+      <c r="O47" s="46">
+        <v>20</v>
+      </c>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="43" cm="1">
+        <f t="array" ref="Q47:Q51">S33-MMULT(AA24:AE28,P40:P44+Q40:Q44)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M48" s="17">
+        <v>18</v>
+      </c>
+      <c r="N48" s="17">
+        <v>4</v>
+      </c>
+      <c r="O48" s="46">
+        <v>20</v>
+      </c>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="17">
+        <v>18</v>
+      </c>
+      <c r="N49" s="17">
+        <v>10</v>
+      </c>
+      <c r="O49" s="46">
+        <v>20</v>
+      </c>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="M50" s="17">
+        <v>18</v>
+      </c>
+      <c r="N50" s="17">
+        <v>6</v>
+      </c>
+      <c r="O50" s="46">
+        <v>20</v>
+      </c>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="M51" s="17">
+        <v>18</v>
+      </c>
+      <c r="N51" s="17">
+        <v>0</v>
+      </c>
+      <c r="O51" s="46">
+        <v>20</v>
+      </c>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O52" s="45"/>
+      <c r="P52" s="10"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M53" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" s="17" cm="1">
+        <f t="array" ref="M54:O58">M24:O28*M35:O35</f>
+        <v>0</v>
+      </c>
+      <c r="N54" s="17">
+        <v>0</v>
+      </c>
+      <c r="O54" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="M55" s="17">
+        <v>0</v>
+      </c>
+      <c r="N55" s="17">
+        <v>2</v>
+      </c>
+      <c r="O55" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="M56" s="17">
+        <v>0</v>
+      </c>
+      <c r="N56" s="17">
+        <v>6</v>
+      </c>
+      <c r="O56" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="M57" s="17">
+        <v>0</v>
+      </c>
+      <c r="N57" s="17">
+        <v>4</v>
+      </c>
+      <c r="O57" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="M58" s="17">
+        <v>0</v>
+      </c>
+      <c r="N58" s="17">
+        <v>0</v>
+      </c>
+      <c r="O58" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>